<commit_message>
feat(epic_app/importers/xlsx_question_importer.py): Fixed question importer to include the group as a filtering condition
</commit_message>
<xml_diff>
--- a/backend/epic_app/tests/test_data/xlsx/initial_epic_data.xlsx
+++ b/backend/epic_app/tests/test_data/xlsx/initial_epic_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\repos\EPIC-Tool\backend\epic_app\tests\test_data\xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8B357F6-B743-4630-821C-B428A62993FB}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD921727-74AD-49C4-955A-6F51D50BD1B5}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="576" yWindow="600" windowWidth="21600" windowHeight="11340" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="480" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="initial_epic_data" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="105">
   <si>
     <t>EPIC elements</t>
   </si>
@@ -394,9 +394,6 @@
   </si>
   <si>
     <t>TBD: Respond Flood Monitoring</t>
-  </si>
-  <si>
-    <t>TBD: Epic</t>
   </si>
   <si>
     <t>Water Resource Management</t>
@@ -1252,19 +1249,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="A42" sqref="A42"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.88671875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="55.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="46.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="255.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="55.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="46.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="255.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1278,7 +1275,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -1286,13 +1283,13 @@
         <v>5</v>
       </c>
       <c r="C2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -1300,13 +1297,13 @@
         <v>5</v>
       </c>
       <c r="C3" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D3" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -1320,7 +1317,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -1334,7 +1331,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -1348,7 +1345,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>4</v>
       </c>
@@ -1362,7 +1359,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>4</v>
       </c>
@@ -1376,7 +1373,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>4</v>
       </c>
@@ -1390,7 +1387,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>4</v>
       </c>
@@ -1404,7 +1401,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>4</v>
       </c>
@@ -1418,7 +1415,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>4</v>
       </c>
@@ -1432,7 +1429,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>4</v>
       </c>
@@ -1446,7 +1443,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>4</v>
       </c>
@@ -1460,7 +1457,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>4</v>
       </c>
@@ -1474,7 +1471,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>4</v>
       </c>
@@ -1488,7 +1485,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>4</v>
       </c>
@@ -1502,7 +1499,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>38</v>
       </c>
@@ -1516,7 +1513,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>38</v>
       </c>
@@ -1530,7 +1527,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>38</v>
       </c>
@@ -1544,7 +1541,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>38</v>
       </c>
@@ -1558,7 +1555,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>38</v>
       </c>
@@ -1572,7 +1569,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>50</v>
       </c>
@@ -1586,7 +1583,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>50</v>
       </c>
@@ -1600,7 +1597,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>50</v>
       </c>
@@ -1614,7 +1611,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>50</v>
       </c>
@@ -1628,7 +1625,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>50</v>
       </c>
@@ -1642,7 +1639,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>50</v>
       </c>
@@ -1656,7 +1653,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>50</v>
       </c>
@@ -1670,7 +1667,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>50</v>
       </c>
@@ -1684,7 +1681,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>69</v>
       </c>
@@ -1698,7 +1695,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>69</v>
       </c>
@@ -1712,7 +1709,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>69</v>
       </c>
@@ -1726,7 +1723,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>69</v>
       </c>
@@ -1740,7 +1737,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>69</v>
       </c>
@@ -1754,7 +1751,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>81</v>
       </c>
@@ -1768,7 +1765,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>81</v>
       </c>
@@ -1782,7 +1779,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>81</v>
       </c>
@@ -1796,7 +1793,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>81</v>
       </c>
@@ -1810,7 +1807,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>81</v>
       </c>
@@ -1824,7 +1821,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>81</v>
       </c>
@@ -1838,9 +1835,9 @@
         <v>94</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>103</v>
+        <v>81</v>
       </c>
       <c r="B42" s="1" t="s">
         <v>91</v>
@@ -1852,7 +1849,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>81</v>
       </c>
@@ -1866,7 +1863,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>81</v>
       </c>
@@ -1887,9 +1884,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2122,19 +2122,15 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{15E7E575-14AC-46DC-BAE5-057A9DA98469}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{474350AB-95E6-4F06-8DEF-D46722A2A1B6}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -2159,9 +2155,10 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{474350AB-95E6-4F06-8DEF-D46722A2A1B6}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{15E7E575-14AC-46DC-BAE5-057A9DA98469}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
ci(initial_epic_data.xlsx): Updated domain data
</commit_message>
<xml_diff>
--- a/backend/epic_app/tests/test_data/xlsx/initial_epic_data.xlsx
+++ b/backend/epic_app/tests/test_data/xlsx/initial_epic_data.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\repos\EPIC-Tool\backend\epic_app\tests\test_data\xlsx\_new\originals\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\repos\EPIC-Tool\backend\epic_app\tests\test_data\xlsx\originals\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45B47D00-3B4B-4EBC-ACBD-8F6CAE8F9E7B}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB2AC24F-C7F6-4BEF-93D0-323F2721EAF2}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11664" yWindow="1272" windowWidth="11376" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-8190" yWindow="6330" windowWidth="16800" windowHeight="11325" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="initial_epic_data" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="128">
   <si>
     <t>EPIC elements</t>
   </si>
@@ -380,6 +380,187 @@
 Flood Forecasting and Warning: Different types of flood require different approaches. Flood forecasts and warning require a cooperation nexus among the NMS/NHS, WRM, and DRM agencies. Clear interagency agreements and operational protocols need to be developed to ensure that this nexus operates efficiently. One option is to establish a National Flood Center which can foster collaboration and flexibility to handle a variety of floods. 
 Agrometeorological Advisory Services: Farmers are particularly prone to be affected by fluctuations in weather and by extreme hydro-climatic events, particularly droughts. It is estimated that 20-80 percent of the inter-annual variability of crop yields is associated with weather phenomena, and 5-10 percent of national agricultural production losses are associated with climate variability. NMS/NHS can team with agriculture agencies to help farmers better cope with climate variability and extreme events through the provision of agro-climate advisory services. Farmers receive information at different time scales to help them make informed decisions. For example, weather forecasts up to a week in advance can help them make decisions regarding planting and harvesting, fertilizer application, and irrigation requirements. Seasonal forecasts on the order of months can inform cropping decisions and livestock strategies. 
 National Climate Assessment helps to inform the country about already observed changes, the current status of the climate, and anticipated trends for the future.  It typically provides analysis of the effects of climate change on the environment, agriculture, health, water resources, and coastal areas, and includes an analysis of flood and drought risks. An NCA can help guide adaptation actions across society by informing planning at all levels, influencing private investment decisions, and spurring actions to enhance climate resilience. The development of an NCA needs to be a collaborative effort with many national agencies, as well as other stakeholders. Although lead responsibility for the formulation of an NCA will vary by country, in every case the NMS/NHS needs to be front-and-center in the process as the leading authority on climate. </t>
+  </si>
+  <si>
+    <t>Key resources</t>
+  </si>
+  <si>
+    <t xml:space="preserve">•	Gencer, Ebru A., and UNISDR (United Nations Office for Disaster Risk Reduction). 2017. Local Government Powers for Disaster Risk Reduction: A Study on Local-level Authority and Capacity for Resilience. UNISDR.
+•	GFDRR (Global Facility for Disaster Reduction and Recovery). 2019. Guide to Engaging Local Actors in Disaster Recovery Frameworks. Washington, DC: World Bank. 
+•	ICLEI (Local Governments for Sustainability). 2008. Local Government and Integrated Water Resources Management (IWRM): Parts I-IV. Freiburg: ICLEI. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">•	EPA (U.S. Environmental Protection Agency). 2018. “Public Participation Guide in Multiple Languages.” February 22, 2018. https://www.epa.gov/international-cooperation/public-participation-guide.
+•	FEMA (Federal Emergency Management Agency). 2011. A Whole Community Approach to Emergency Management: Principles, Themes, and Pathways for Action. Washington, DC: FEMA. 
+•	GWP (Global Water Partnership). 2017. “IWRM Toolbox: C5 Communication.” March 31, 2017. 
+•	IAP2 (International Association of Public Participation). n.d. “Advancing the practice of public participation.” </t>
+  </si>
+  <si>
+    <t xml:space="preserve">•	Erman, Alvina, Sophie Anne De Vries Robbe, Stephan Fabian Thies, Kayenat Kabir, and Mirai Maruo. 2021. Gender Dimensions of Disaster Risk and Resilience: Existing Evidence. World Bank,
+•	IFRC (International Federation of Red Cross and Red Crescent Societies). 2012. Community Early Warning Systems: Guiding Principles. Geneva: IFRC.
+•	IRC (International Water and Sanitation Centre).2019. Quick Scan of Socially Inclusive Integrated Water Resources Management. IRC: The Hague.
+•	Meijer, Karen, Caroline Sullivan, Judith Blaauw, Femke Schasfoort, Bouke Ottow, and Diana Morales. 2019. “Social Inclusiveness in Floods and Droughts: How Social Variations in Impacts and Responses Can Be Taken into Account.” Working Paper, Deltares, Delft. 
+•	UNESCO (United Nations Educational, Scientific and Cultural Organization). 2015. “Reinforcing the Resilience of Indigenous Peoples and Sharing Knowledge to Address Climate Change.” November 26, 2015. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">•	OECD (Organisation for Economic Co-operation and Development). 2016. Trends in Risk Communication Policies and Practices. OECD Reviews of Risk Management Policies. Paris: OECD Publishing. 
+•	Shaw, Chris and Adam Corner. 2014. Communicating Drought Risk in A Changing Climate. Oxford: Climate Outreach. 
+•	WMO (World Meteorological Organization) and GWP CEE (Global Water Partnership Central and Eastern Europe). 2019. How to Communicate Drought: A guide by the Integrated Drought Management Programme in Central and Eastern Europe, 2019. Geneva: WMO. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">•	Daniels, Elizabeth, Sukaina Bharwani, Åsa Gerger Swartling, Gregor Vulturius, Karen Brandon. 2020. “Refocusing the climate services lens: Introducing a framework for co-designing “transdisciplinary knowledge integration processes” to build climate resilience.” Climate Services 19 (100181). </t>
+  </si>
+  <si>
+    <t>•	EU (European Commission). 2011. Communication from the Commission to the European Parliament, the Council, the European Economic and Social Committee and the Committee of the Regions. “Open data: An engine for innovation, growth and transparent governance.”
+•	EU (European Commission). 2019. “EU Directive 2019/1024 of the European Parliament and of the Council of 20 June 2019 on open data and the re-use of public sector information.” OJ L 172, 26.6.2019, p. 56. 
+•	GSA (U.S. General Services Administration). n.d. “Federal Crowdsourcing and Citizen Science Toolkit.” 
+•	World Bank. 2019. “Open Government Data Toolkit.” Washington, DC: World Bank.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">•	Rogers, David P., and Vladimir V. Tsirkunov. 2010. Global Assessment Report on Disaster Risk Reduction: Costs and Benefits of Early Warning Systems. United Nations International Strategy for Disaster Reduction (UNISDR) and World Bank. 
+•	Rogers, David P., and Vladimir V. Tsirkunov. 2013. Weather and Climate Resilience: Effective Preparedness through National Meteorological and Hydrological Services. Directions in Development. Washington, DC: World Bank. 
+•	Rogers David P., Vladimir V. Tsirkunov, Haleh Kootval, Alice Soares, Daniel Kull, Anna-Maria Bogdanov, and Makoto Suwa. 2019. Weathering the Change: How to Improve Hydromet Services in Developing Countries. Washington, DC: World Bank. 
+•	World Bank. 2019.The Power of Partnership: Public and Private Engagement on Hydromet Services. Washington, DC: World Bank. 
+•	WMO (World Meteorological Organization). 2015. “WMO guidelines on multi-hazard impact-based forecast and warning services.” WMO TD no. 1150. 
+•	WMO (World Meteorological Organization), World Bank, and USAID (United States Agency for International Development). 2015. Valuing Weather and Climate: Economic Assessment of Meteorological and Hydrological Services. Geneva: WMO. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">•	Van Beek, Eelco, and others. (Forthcoming). Analysis Framework for Water Resources Planning and Implementation. Delft: Deltares.
+•	GWP (Global Water Partnership), and INBO (International Network of Basin Organizations). 2009. A Handbook for Integrated Water Resources Management in Basins. Stockholm: GWP; Paris: INBO. 
+•	GWP CEE (Global Water Partnership Central and Eastern Europe) and WMO (World Meteorological Organization). 2015. Guidelines for Preparation of Drought Management Plans: Development and Implementation in the Context of the EU Water Framework Directive. Bratislava: GWP CEE. 
+•	Sayers, Paul, Li Yuanyuan, Gerald Galloway, Edmund Penning-Rowsell, Fuxin Shen, Wen Kang, Chen Yiwei, and Tom Le Quesne. 2013. Flood Risk Management: A Strategic Approach. ADB (Asian Development Bank), WWF-UK (World Wildlife Fund), GIWP (General Institute of Water Resources and Hydropower Planning and Design), and UNESCO (United Nations Educational, Scientific and Cultural Organization). </t>
+  </si>
+  <si>
+    <t xml:space="preserve">•	FAO (Food &amp; Agriculture Organization of the United Nations). 2006. Integrated Coastal Management Law: Establishing and Strengthening National Legal Frameworks for Integrated Coastal Management. FAO Legislative Study 93. Rome: FAO. 
+•	NOAA (National Oceanic and Atmospheric Administration). 2018. National Coastal Zone Management Program: Strategic Plan 2018-2023. Washington, DC: NOAA. 
+•	Post, Jan C., and Carl G. Lundin, eds. 1996. Guidelines for Integrated Coastal Zone Management. Washington, DC: World Bank. 
+•	USAID (U.S. Agency for International Development). 2009. Adapting to Coastal Climate Change: A Guidebook for Development Planners. Washington DC: USAID. 
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">•	AWWA (American Water Works Association). 2017. M50 Water Resources Planning, 3rd ed. Manual of Water Supply Practices. Denver: AWWA.
+•	AWWA (American Water Works Association). 2019. M60 Drought Preparedness and Response, 2nd ed. Manual of Water Supply Practices. Denver: AWWA.
+•	California Department of Water Resources. 2008. Urban Drought Guidebook. Sacramento: California Department of Water Resources. </t>
+  </si>
+  <si>
+    <t>•	California Department of Agriculture. 2015. Agricultural Water Management Plan Guidebook. Sacramento: California Department of Agriculture. 
+•	OECD (Organization for Economic Co-operation and Development). 2016. Mitigating Droughts and Floods in Agriculture: Policy Lessons and Approaches. OECD Studies on Water. Paris: OECD.  
+ </t>
+  </si>
+  <si>
+    <t xml:space="preserve">•	CCAFS (Consultative Group on International Agricultural Research (CGIAR) Program on Climate Change, Agriculture and Food Security). 2020. “Climate Smart Agriculture.” 
+•	FAO (Food and Agriculture Organization of the United Nations). 2017. Voluntary Guidelines for Sustainable Soil Management. Rome: FAO. 
+•	Liniger, Hanspeter, and Rima Mekdaschi Studer. 2019. Sustainable Rangeland Management in Sub-Saharan Africa: Guidelines to Good and Protect Our Waters. TerrAfrica Partnership. Washington, DC: World Bank; Bern: WOCAT (World Overview of Conservation Approaches and Technologies); Bern: CDE (Centre for Development and Environment, University of Bern). 
+•	NRCS (U.S. Natural Resources Conservation Service). 2020. “Conservation Practice Standards.” Washington, DC: NRCS. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">•	FAO (Food and Agriculture Organization of the United Nations). 2020. “Sustainable Forestry Management for Soil and Water Conservation.” November 4, 2020. 
+•	Spalding, Mark Douglas, Anna Mcivor, Femke H. Tonneijck, Susanna Tol, and Pieter van Eijk. 2014. Mangroves for Coastal Defence: Guidelines for Coastal Managers &amp; Policy Makers. Wageningen: Wetlands International; Arlington: Nature Conservancy. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">•	GWP (Global Water Partnership), and WMO (World Meteorological Organization). 2012. Conservation and Restoration of Rivers and Floodplains. Integrated Flood Management Tools Series no.13. 
+•	Ramsar Convention Secretariat. 2010. Laws and Institutions: Reviewing Laws and Institutions to Promote the Conservation and Wise Use of Wetlands. Ramsar Handbooks for the Wise Use of Wetlands, 4th ed. vol.3. Gland: Ramsar Convention Secretariat. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">•	Darghouth, Salah, Christopher Ward, Gretel Gambarelli, Erika Styger, and Julienne Roux. 2008. “Watershed Management Approaches, Policies, and Operations: Lessons for Scaling Up.” Water Sector Board Discussion Paper Series no. 11. Washington, DC: World Bank. 
+•	EPA (U.S. Environmental Protection Agency). 2013. A Quick Guide to Developing Watershed Plans to
+•	Restore and Protect Our Waters. Washington, DC: EPA. 
+•	Mathews, Ruth. E., Anna Tengberg, Johanna Sjödin, and Brigitta Liss-Lymer. 2019. Implementing the Source-to-Sea Approach: A Guide for Practitioners. Stockholm: SIWI (Stockholm International Water Institute).
+•	UNESCO (United Nations Educational, Scientific and Cultural Organization). 2018. World Water Development Report 2018: Nature-Based Solutions for Water. Paris: UNESCO. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">•	OECD (Organisation for Economic Co-operation and Development). 2012. A Framework for Financing Water Resources Management. Paris: OECD. 
+•	OECD (Organisation for Economic Co-operation and Development). 2017. “Multi-Purpose Water Infrastructure: Recommendations to Maximise Economic Benefits.” OCDE Policy Perspectives. Paris: OCDE. 
+•	US CEQ (U.S. Council on Environmental Quality). 2013. Principles and Requirements for Federal Investments in Water Resources. Washington, DC: CEQ. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">•	ICOLD (International Commission on Large Dams). 2014. “Regulation of Dam Safety: An Overview of Current Practice Worldwide.” Technical Bulletin no. 167. Paris: ICOLD/CIGB.
+•	ICOLD (International Commission on Large Dams). 2019. World Declaration on Dam Safety: Better Dams for a Better World. Porto: ICOLD. 
+•	Wishart, Marcus J., Satoru Ueda, John D. Pisaniello, Joanne L. Tingey-Holyoak, Kimberly N. Lyon, and Esteban Boj García. 2020. “Laying the Foundations: A Global Analysis of Regulatory Frameworks for the Safety of Dams and Downstream Communities.” Sustainable Infrastructure Series. Washington, DC: World Bank. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">•	CIRIA (Construction Industry Research and Information Association). 2013. The International Levee Handbook. London: CIRIA.
+•	U.S. National Committee on Levee Safety. 2011. Creating a National Levee Safety Program: Recommendations from the National Committee on Levee Safety. Washington, DC: U.S. National Committee on Levee Safety. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">•	FAO (Food and Agriculture Organization of the United Nations). 2006. Modern Water Rights: Theory and Practice. Rome: FAO. 
+•	GWP (Global Water Partnership). 2019. “Sharing Water: The Role of Robust Water-Sharing Arrangements in Integrated Water Resources Management.” Perspectives Paper. Stockholm: GWP. 
+•	OECD (Organization for Economic Co-operation and Development). 2015. Water Resources Allocation: Sharing Risks and Opportunities. OECD Studies on Water. Paris: OECD. 
+•	OECD (Organization for Economic Co-operation and Development). 2016. Mitigating Droughts and Floods in Agriculture: Policy Lessons and Approaches. OECD Studies on Water. Paris: OECD. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">•	FAO (Food &amp; Agriculture Organization of the United Nations). 2016. Global Framework for Action to Achieve the Vision on Groundwater Governance. Rome: FAO. 
+•	Kresic, Neven. 2009. Groundwater Resources: Sustainability, Management, and Restoration. New York: McGraw-Hill. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">•	FEMA (Federal Emergency Management Agency). 2020. “Risk Mapping, Assessment and Planning (Risk MAP).” FEMA, December 17, 2020. 
+•	Martini, Frederique, and Roberto Loat. 2007. Handbook on Good Practices for Flood Mapping in Europe. Paris/Bern: European Exchange Circle on Flood Mapping (EXCIMAP). 
+•	WMO (World Meteorological Organization) and GWP (Global Water Partnership). 2013. “Flood Mapping. Integrated Flood Management Tool Series.” Technical Document no. 20. Geneva: WMO. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">•	Association of State Floodplain Managers (https://www.floods.org).
+•	FEMA (Federal Emergency Management Agency). 2009. A Local Administrator’s Guide to Floodplain Management and the National Flood Insurance Program. Washington, DC: FEMA. 
+•	FEMA (Federal Emergency Management Agency). 2018. Flood Resistant Provisions of the 2018 International Codes. Washington, DC: FEMA, 
+•	WMO (World Meteorological Organization) and GWP (Global Water Partnership). 2016. “The Role of Land Use Planning in Flood Management.” Integrated Flood Management Tool Series, Technical Document no. 7. Geneva: WMO. </t>
+  </si>
+  <si>
+    <t>•	AIDR (Australian Institute for Disaster Resilience). 2013. Managing the Flood Plain: A Guide to Best Practice in Flood Risk Management in Australia. East Melbourne: AIDR. 
+•	FEMA (Federal Emergency Management Agency). 2013. Local Mitigation Planning Handbook. Washington, DC: FEMA.
+•	WMO (World Meteorological Organization) and GWP (Global Water Partnership). 2017. “Selecting Measures and Designing Strategies for Integrated Flood Management: A Guidance Document.” Policy and Tools Documents Series no.1 version 1.0. Geneva: WMO. 
+ </t>
+  </si>
+  <si>
+    <t xml:space="preserve">•	IDMP (Integrated Drought Management Programme). 2018. “Integrated Drought Management HelpDesk.” 
+•	NDMC (National Drought Mitigation Center). 2021. “United States Drought Monitor.” NDMC.
+•	NIDIS (National Integrated Drought Information System). 2007.The National Integrated Drought Information System Implementation Plan: A Pathway for National Resilience. 
+•	World Bank. 2019. Assessing Drought Hazard and Risk: Principles and Implementation Guidance. Washington, DC: The World Bank. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">•	Lesk, Cory, Pedram Rowhani, and Navin Ramankutty. 2016. “Inﬂuence of Extreme Weather Disasters on Global Crop production.” Nature 529 (7584): 84–87. 
+•	Mahul, Olivier, and Charles J. Stutley. 2010. Government Support to Agricultural Insurance: Challenges and Options for Developing Countries. Washington, DC: World Bank. 
+•	Raithatha, Rishi, and Priebe Jan. 2020. Agricultural insurance for smallholder farmers: Digital Innovations for Scale. GSMA AgriTech Programme. 
+•	Reyes, Celia M., Adrian D. Agbon, Christian D. Mina, and Ann B. Reneli Gloria. 2017. “Agricultural Insurance Program: Lessons from Different Country Experiences.” PIDS Discussion Paper Series no. 2017-02. Quezon City: Philippine Institute for Development Studies. 
+•	Sandmark, Thérèse, Jean-Christophe Debar, and Clémence Tatin-Jaleran. 2013. “The Emergence and Development of Agriculture Microinsurance.” A Discussion Paper. Luxembourg: Microinsurance Network.
+•	USDA (United States Department of Agriculture). 2017. Disaster Assistance Fact Sheet. Washington, DC: USDA. </t>
+  </si>
+  <si>
+    <t>•	Lindert, Kathy, Tina George Karippacheril, Inés Rodriguez Caillava, and Kenichi Nishikawa Chavez. 2020. Sourcebook on the Foundations of Social Protection Delivery Systems. Washington, DC: World Bank. 
+•	Monchuk, Victoria. 2014. Reducing poverty and investing in people. The new role of safety nets in Africa. Directions in Development. Washington, DC: World Bank. 
+•	Pelham, Larissa, Edward Clay, and Tim Braunholz. 2011. “Natural Disasters: What is the Role for Social Safety Nets?” World Bank Social Protection Discussion Paper no. 1102. Washington, DC: World Bank.</t>
+  </si>
+  <si>
+    <t>•	FEMA (U.S. Federal Emergency Management Agency). 2020. “Hurricane Planning and Response.” FEMA, July 23, 2020. 
+•	GWP (Global Water Partnership) and WMO (World Meteorological Organization). 2013. “Flood Forecasting and Early Warning.” Integrated Flood Management Tools Series, Technical Document no. 19. Geneva: WMO.
+•	Rogers, David P, and Vladimir V. Tsirkunov. 2013. Weather and Climate Resilience: Effective Preparedness through National Meteorological and Hydrological Services. Directions in Development. Washington, DC: World Bank. 
+•	WMO (World Meteorological Organization). n.d. “Storm Surges.” https://public.wmo.int/en/our-mandate/focus-areas/natural-hazards-and-disaster-risk-reduction/storm-surge.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">•	CalOES (California Governor’s Office of Emergency Services). 2017. State of California Emergency Plan. Sacramento: California Governor’s Office of Emergency Services. 
+•	DHS (U.S. Department of Homeland Security). 2019. National Response Framework. 4th ed. Washington, DC: DHS. 
+•	EU (European Commission), UNDG (United Nations Development Group), and GFDRR (Global Facility for Disaster Reduction and Recovery). 2013. Post-Disaster Needs Assessments. Volume A: Guidelines. Brussels: EU. 
+•	FEMA (U.S. Federal Emergency Management Agency). 2010. Developing and Maintaining Emergency Operations Plans. Comprehensive Preparedness Guide (CPG) Version 2.0. Washington, DC.
+•	FEMA (U.S. Federal Emergency Management Agency). 2017. Principles of Emergency Management. Washington, DC: FEMA.
+•	Gilissen, Herman Kasper, Alexander Meghan, Piotr Matczak, Maria Pettersson, and Silvia Bruzzone. 2016. “A Framework for Evaluating the Effectiveness of Flood Emergency Management Systems in Europe.” Ecology and Society 21 (4):27. 
+•	Pelham, Larissa, Edward Clay, and Tim Braunholz. 2011. “Natural Disasters: What is the Role for Social Safety Nets?” World Bank Social Protection Discussion Paper no. 1102. Washington, DC: World Bank.
+•	WMO (World Meteorological Organization) and GWP (Global Water Partnership). 2011. “Flood Emergency Planning.” Integrated Flood Management Tools Series, Technical Document no. 11. Geneva: WMO. </t>
+  </si>
+  <si>
+    <t>•	APA (American Planning Association). 2014. Planning for Post-Disaster Recovery: Next Generation. Chicago: APA Planning Advisory Service.
+•	EU (European Commission), UNDG (United Nations Development Group), and GFDRR (Global Facility for Disaster Reduction and Recovery). 2013. Post-Disaster Needs Assessments. Volume B: Guidelines. Brussels: EU. 
+•	GFDRR (Global Facility for Disaster Reduction and Recovery). 2015. Guide to Developing Disaster Recovery Frameworks: Sendai Conference Version. Washington, DC: World Bank. 
+•	Hallegatte, Stephane, Jun Rentschler, and Brian Walsh. 2018. Building Back Better: Achieving Resilience through Stronger, Faster, and More Inclusive Post-Disaster Reconstruction. Washington, DC: GFDRR (Global Facility for Disaster Reduction and Recovery). 
+•	IFRC (International Federation of Red Cross and Red Crescent Societies). 2012. Post-Disaster Community Infrastructure Rehabilitation and (Re)construction Guidelines. Geneva: IFRC. 
+•	Jha, Abhas K., Jennifer Duyne Barenstein, Priscilla M. Phelps, Daniel Pittet, and Stephen Sena. 2010. Safer Homes, Stronger Communities: A Handbook for Reconstruction after Natural Disasters. Washington, DC: World Bank. 
+•	OECD (Organization for Economic Co-operation and Development). 2016. Financial Management of Flood Risk. Paris: OECD. 
+•	US Congressional Research Office. 2012. Introduction to the National Flood Insurance Program (NFIP). Washington, DC: US Congressional Research Office.</t>
+  </si>
+  <si>
+    <t>•	ADB (Asian Development Bank). 2018. “Catastrophe Bonds Explained.” Development Asia. February 21, 2018. 
+•	Benson, Charlotte, Olivier Mahul, Martin Luis Alton. 2017. “Assessing Financial Protection against Disasters: A Guidance Note on Conducting a Disaster Risk Finance Diagnostic.” Working Paper. Washington, DC: World Bank; Manila: ADB (Asian Development Bank). 
+•	GFDRR (Global Facility for Disaster Reduction and Recovery). n.d. “Financial protection: Strengthening Financial Resilience to Disasters.” (https://www.gfdrr.org/en/financial-protection.)
+•	OECD (Organization for Economic Co-operation and Development). 2017. OECD Recommendations on Disaster Risk Financing Strategies. Paris: OECD. 
+•	World Bank. 2017. “Catastrophe Deferred Drawdown.” Product Note. Washington, DC: World Bank. 
+•	World Bank. 2020. “Technical Note on Agricultural Risk Financing Options for World Bank Group Operations.” Washington, DC: World Bank.</t>
   </si>
 </sst>
 </file>
@@ -1222,22 +1403,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D45"/>
+  <dimension ref="A1:E40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A30" workbookViewId="0">
-      <selection activeCell="A38" sqref="A38"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="55.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="46.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="255.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="16384" width="9.109375" style="1"/>
+    <col min="1" max="1" width="13.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="55.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="46.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="58.7109375" style="1" hidden="1" customWidth="1"/>
+    <col min="5" max="5" width="24.42578125" style="1" customWidth="1"/>
+    <col min="6" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1250,8 +1432,11 @@
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E1" s="1" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
@@ -1265,7 +1450,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
@@ -1279,7 +1464,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>4</v>
       </c>
@@ -1293,7 +1478,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
@@ -1307,7 +1492,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
@@ -1320,8 +1505,11 @@
       <c r="D6" s="1" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E6" s="1" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>4</v>
       </c>
@@ -1334,8 +1522,11 @@
       <c r="D7" s="1" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E7" s="1" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>4</v>
       </c>
@@ -1348,8 +1539,11 @@
       <c r="D8" s="1" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E8" s="1" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>4</v>
       </c>
@@ -1362,8 +1556,11 @@
       <c r="D9" s="1" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E9" s="1" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>4</v>
       </c>
@@ -1376,8 +1573,11 @@
       <c r="D10" s="1" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E10" s="1" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>4</v>
       </c>
@@ -1390,8 +1590,11 @@
       <c r="D11" s="1" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E11" s="1" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>4</v>
       </c>
@@ -1404,8 +1607,11 @@
       <c r="D12" s="1" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E12" s="1" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>4</v>
       </c>
@@ -1418,8 +1624,11 @@
       <c r="D13" s="1" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E13" s="1" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>16</v>
       </c>
@@ -1432,8 +1641,11 @@
       <c r="D14" s="1" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E14" s="1" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>16</v>
       </c>
@@ -1446,8 +1658,11 @@
       <c r="D15" s="1" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E15" s="1" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>16</v>
       </c>
@@ -1460,8 +1675,11 @@
       <c r="D16" s="1" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E16" s="1" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>16</v>
       </c>
@@ -1474,8 +1692,11 @@
       <c r="D17" s="1" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E17" s="1" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>16</v>
       </c>
@@ -1488,8 +1709,11 @@
       <c r="D18" s="1" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E18" s="1" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>23</v>
       </c>
@@ -1502,8 +1726,11 @@
       <c r="D19" s="1" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E19" s="1" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>23</v>
       </c>
@@ -1516,8 +1743,11 @@
       <c r="D20" s="1" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E20" s="1" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>23</v>
       </c>
@@ -1530,8 +1760,11 @@
       <c r="D21" s="1" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E21" s="1" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>23</v>
       </c>
@@ -1544,8 +1777,11 @@
       <c r="D22" s="1" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E22" s="1" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>23</v>
       </c>
@@ -1558,8 +1794,11 @@
       <c r="D23" s="1" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E23" s="1" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>23</v>
       </c>
@@ -1572,8 +1811,11 @@
       <c r="D24" s="1" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E24" s="1" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>23</v>
       </c>
@@ -1586,8 +1828,11 @@
       <c r="D25" s="1" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E25" s="1" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>23</v>
       </c>
@@ -1600,8 +1845,11 @@
       <c r="D26" s="1" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E26" s="1" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>34</v>
       </c>
@@ -1614,8 +1862,11 @@
       <c r="D27" s="1" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E27" s="1" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>34</v>
       </c>
@@ -1628,8 +1879,11 @@
       <c r="D28" s="1" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E28" s="1" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>34</v>
       </c>
@@ -1642,8 +1896,11 @@
       <c r="D29" s="1" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E29" s="1" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>34</v>
       </c>
@@ -1656,8 +1913,11 @@
       <c r="D30" s="1" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E30" s="1" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>34</v>
       </c>
@@ -1670,8 +1930,11 @@
       <c r="D31" s="1" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E31" s="1" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>42</v>
       </c>
@@ -1684,8 +1947,11 @@
       <c r="D32" s="1" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E32" s="1" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>42</v>
       </c>
@@ -1699,7 +1965,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
         <v>42</v>
       </c>
@@ -1712,8 +1978,11 @@
       <c r="D34" s="1" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E34" s="1" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
         <v>42</v>
       </c>
@@ -1726,8 +1995,11 @@
       <c r="D35" s="1" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E35" s="1" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
         <v>42</v>
       </c>
@@ -1740,8 +2012,11 @@
       <c r="D36" s="2" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E36" s="1" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
         <v>42</v>
       </c>
@@ -1754,8 +2029,11 @@
       <c r="D37" s="2" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E37" s="1" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
         <v>42</v>
       </c>
@@ -1768,8 +2046,11 @@
       <c r="D38" s="2" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E38" s="1" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
         <v>42</v>
       </c>
@@ -1782,8 +2063,11 @@
       <c r="D39" s="1" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E39" s="1" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
         <v>42</v>
       </c>
@@ -1796,9 +2080,9 @@
       <c r="D40" s="1" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="D45"/>
+      <c r="E40" s="1" t="s">
+        <v>127</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1807,6 +2091,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101004CF95EF2F384F0419312B394CBDE3AE2" ma:contentTypeVersion="14" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="31f6efdc87a01d4ba6154ecd9afe69b2">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="18fba281-3140-4e33-b78f-87df0c1efb23" xmlns:ns4="f7620e32-1325-4c29-861c-5840d24c4310" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="ef933d5bbd2bd3eb58c8ad997b164a29" ns3:_="" ns4:_="">
     <xsd:import namespace="18fba281-3140-4e33-b78f-87df0c1efb23"/>
@@ -2035,15 +2328,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
@@ -2051,6 +2335,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{474350AB-95E6-4F06-8DEF-D46722A2A1B6}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B1E28E4C-E1CF-40DF-A02F-65C5F89D9385}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2065,14 +2357,6 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{474350AB-95E6-4F06-8DEF-D46722A2A1B6}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>